<commit_message>
Upload File Creation Properties
</commit_message>
<xml_diff>
--- a/UTIL.FILE.HELPER/CRM.CONTACTS.XREF.xlsx
+++ b/UTIL.FILE.HELPER/CRM.CONTACTS.XREF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matttownsend/Development/qm/dev/UTIL.FILE.HELPER/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2505C62-CFE2-904E-90CD-07EE03BA6C50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C26D0A-5F4A-7A45-8417-514DA5887B69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4580" yWindow="5800" windowWidth="20460" windowHeight="11040" xr2:uid="{813E0F8E-BFCA-4822-954C-5BA9526CDC97}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>Field</t>
   </si>
@@ -72,13 +72,16 @@
     <t>/</t>
   </si>
   <si>
-    <t>DATA</t>
-  </si>
-  <si>
     <t>CTFR</t>
   </si>
   <si>
     <t>CRM.CONTACTS.XREF</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>XREF</t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,7 @@
   <dimension ref="B1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -488,7 +491,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
@@ -503,7 +506,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -555,10 +558,10 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3">
         <v>35</v>
@@ -571,11 +574,11 @@
       </c>
       <c r="I5">
         <f t="shared" ref="I5:I8" si="0">C5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" t="str">
         <f>B5</f>
-        <v>DATA</v>
+        <v>ID</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" ref="L5:L8" si="1">D5&amp;E5</f>
@@ -586,24 +589,32 @@
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>35</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="H6" t="s">
         <v>5</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="str">
         <f t="shared" ref="K6:K8" si="2">B6</f>
-        <v>0</v>
+        <v>XREF</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>35L</v>
       </c>
       <c r="M6" t="s">
         <v>6</v>
@@ -740,13 +751,13 @@
     <row r="4" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C4" s="3" t="str">
         <f>Setup!$C$1&amp;SEPR&amp;Setup!H5&amp;SEPR&amp;Setup!I5&amp;SEPR&amp;Setup!J5&amp;SEPR&amp;Setup!K5&amp;SEPR&amp;Setup!L5&amp;SEPR&amp;Setup!M5&amp;SEPR&amp;Setup!N5</f>
-        <v>CRM.CONTACTS.XREF/D/1//DATA/35L/S/</v>
+        <v>CRM.CONTACTS.XREF/D/0//ID/35L/S/</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C5" s="3" t="str">
         <f>Setup!$C$1&amp;SEPR&amp;Setup!H6&amp;SEPR&amp;Setup!I6&amp;SEPR&amp;Setup!J6&amp;SEPR&amp;Setup!K6&amp;SEPR&amp;Setup!L6&amp;SEPR&amp;Setup!M6&amp;SEPR&amp;Setup!N6</f>
-        <v>CRM.CONTACTS.XREF/D/0//0//S/</v>
+        <v>CRM.CONTACTS.XREF/D/1//XREF/35L/S/</v>
       </c>
     </row>
     <row r="6" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
XREF tables - Build Files
</commit_message>
<xml_diff>
--- a/UTIL.FILE.HELPER/CRM.CONTACTS.XREF.xlsx
+++ b/UTIL.FILE.HELPER/CRM.CONTACTS.XREF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matttownsend/Development/qm/dev/UTIL.FILE.HELPER/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C26D0A-5F4A-7A45-8417-514DA5887B69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F7C991-A970-1443-A564-196DAD529897}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4580" yWindow="5800" windowWidth="20460" windowHeight="11040" xr2:uid="{813E0F8E-BFCA-4822-954C-5BA9526CDC97}"/>
   </bookViews>
@@ -476,7 +476,7 @@
   <dimension ref="B1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>